<commit_message>
excel reading column added
</commit_message>
<xml_diff>
--- a/src/test/java/Data/POIWORK.xlsx
+++ b/src/test/java/Data/POIWORK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResurrectionJavaAug\Resurrection_MyFrameWork2Dec2021\src\test\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{986D7284-BBEC-4BD2-BB4C-ADC5EAEEE1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D975FEBA-386C-4E7F-95E9-0F4685DCFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9D1C48D2-04EE-48BF-A9F1-76A9D823E5CD}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -40,9 +40,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>sumit</t>
   </si>
   <si>
@@ -55,7 +52,22 @@
     <t>pwd2</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>role</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>uft</t>
+  </si>
+  <si>
+    <t>selenium</t>
   </si>
 </sst>
 </file>
@@ -407,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3F31ED-10A9-4683-915B-725B55EDB0FC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,29 +435,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>